<commit_message>
more excel import tests; edit-and-save checks blanks, negative, long strings
git-svn-id: https://svn.fao.org/projects/ruralinvest/RIV4/trunk@66602 d7fa552c-c32d-11e1-9f2d-6d39f2a56844
</commit_message>
<xml_diff>
--- a/RIV4-tests/src/test/resources/imports/project/block.xlsx
+++ b/RIV4-tests/src/test/resources/imports/project/block.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="38">
   <si>
     <t>Sales income</t>
   </si>
@@ -112,9 +112,6 @@
   </si>
   <si>
     <t>Unit type</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>Pilot</t>
@@ -185,11 +182,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -520,13 +518,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <cols>
+    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18">
       <c r="A1" s="2" t="s">
@@ -838,9 +843,7 @@
       <c r="F15" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="G15" s="1"/>
       <c r="H15" s="1" t="s">
         <v>21</v>
       </c>
@@ -850,10 +853,10 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" t="s">
         <v>32</v>
-      </c>
-      <c r="B16" t="s">
-        <v>33</v>
       </c>
       <c r="C16">
         <v>30</v>
@@ -868,6 +871,7 @@
       <c r="F16" s="3">
         <v>15</v>
       </c>
+      <c r="G16" s="4"/>
       <c r="H16" s="3">
         <f>C16*F16</f>
         <v>450</v>
@@ -879,10 +883,10 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C17">
         <v>30</v>
@@ -897,6 +901,7 @@
       <c r="F17" s="3">
         <v>10</v>
       </c>
+      <c r="G17" s="4"/>
       <c r="H17" s="3">
         <f>C17*F17</f>
         <v>300</v>
@@ -921,12 +926,12 @@
     </row>
     <row r="21" spans="1:9" ht="18">
       <c r="G21" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="G22" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H22" s="3">
         <f>H5</f>
@@ -939,7 +944,7 @@
     </row>
     <row r="23" spans="1:9">
       <c r="G23" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H23" s="3">
         <f>H13+H18</f>
@@ -952,7 +957,7 @@
     </row>
     <row r="24" spans="1:9">
       <c r="G24" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H24" s="3">
         <f>H22-H23</f>
@@ -963,9 +968,7 @@
         <v>542.5</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="18"/>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B16:B17">

</xml_diff>